<commit_message>
story 2 test cases
</commit_message>
<xml_diff>
--- a/SSW_555/TeamPraRobSud555.xlsx
+++ b/SSW_555/TeamPraRobSud555.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27907"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basilmajdi\Documents\stevens_SSW\agile methods 555\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sudhansh/git/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="19560" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="198">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -657,19 +657,16 @@
     <t>Not Started</t>
   </si>
   <si>
-    <t xml:space="preserve">coding right now </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jim rowland </t>
-  </si>
-  <si>
     <t xml:space="preserve">bring alchohol; </t>
+  </si>
+  <si>
+    <t>COMPLETED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -824,7 +821,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -882,6 +879,7 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -965,7 +963,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -991,22 +989,22 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41065</c:v>
+                  <c:v>41065.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41078</c:v>
+                  <c:v>41078.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41092</c:v>
+                  <c:v>41092.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41106</c:v>
+                  <c:v>41106.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41120</c:v>
+                  <c:v>41120.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1018,25 +1016,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-AA0F-472A-8A48-BD2444B41C44}"/>
             </c:ext>
@@ -1052,28 +1050,28 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-469478512"/>
-        <c:axId val="-469476192"/>
+        <c:axId val="1116622048"/>
+        <c:axId val="1116624368"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-469478512"/>
+        <c:axId val="1116622048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-469476192"/>
+        <c:crossAx val="1116624368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-469476192"/>
+        <c:axId val="1116624368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1084,7 +1082,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-469478512"/>
+        <c:crossAx val="1116622048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1095,14 +1093,14 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1131,10 +1129,10 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>40442</c:v>
+                  <c:v>40442.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40455</c:v>
+                  <c:v>40455.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1146,16 +1144,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>36</c:v>
+                  <c:v>36.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-17F1-4DF6-AB70-24D0992B24E0}"/>
             </c:ext>
@@ -1171,11 +1169,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-467596544"/>
-        <c:axId val="-467594224"/>
+        <c:axId val="1116664880"/>
+        <c:axId val="1116667632"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-467596544"/>
+        <c:axId val="1116664880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1185,14 +1183,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-467594224"/>
+        <c:crossAx val="1116667632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-467594224"/>
+        <c:axId val="1116667632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1203,7 +1201,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-467596544"/>
+        <c:crossAx val="1116664880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1214,7 +1212,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1240,7 +1238,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1278,7 +1276,7 @@
         <xdr:cNvPr id="3" name="Rectangular Callout 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1353,7 +1351,7 @@
         <xdr:cNvPr id="4" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1418,7 +1416,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1487,7 +1485,7 @@
         <xdr:cNvPr id="6" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1557,7 +1555,7 @@
         <xdr:cNvPr id="7" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1626,7 +1624,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1696,7 +1694,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2043,15 +2041,15 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5" customWidth="1"/>
     <col min="4" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2068,7 +2066,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>181</v>
       </c>
@@ -2085,7 +2083,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>182</v>
       </c>
@@ -2102,7 +2100,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>183</v>
       </c>
@@ -2119,7 +2117,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="D9" s="4" t="s">
         <v>38</v>
       </c>
@@ -2148,16 +2146,16 @@
       <selection activeCell="C2" sqref="C2:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="6.625" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.875" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.875" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.875" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.25" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.83203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.83203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" style="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="B1" s="19" t="s">
         <v>31</v>
       </c>
@@ -2174,7 +2172,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2194,7 +2192,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="24" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" s="24" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2214,7 +2212,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2231,7 +2229,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2248,7 +2246,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2265,7 +2263,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2282,7 +2280,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2296,7 +2294,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2310,7 +2308,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2324,7 +2322,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2353,47 +2351,47 @@
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="7"/>
+    <col min="1" max="1" width="11" style="7"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>166</v>
       </c>
@@ -2416,7 +2414,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>167</v>
       </c>
@@ -2432,7 +2430,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>168</v>
       </c>
@@ -2457,7 +2455,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="7" t="s">
         <v>169</v>
       </c>
@@ -2482,7 +2480,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
         <v>170</v>
       </c>
@@ -2507,7 +2505,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
         <v>171</v>
       </c>
@@ -2547,17 +2545,17 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="2"/>
-    <col min="2" max="2" width="16.625" customWidth="1"/>
+    <col min="1" max="1" width="11" style="2"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="7.125" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2577,7 +2575,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>40442</v>
       </c>
@@ -2588,7 +2586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>40455</v>
       </c>
@@ -2622,21 +2620,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.625" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
     <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.625" customWidth="1"/>
-    <col min="5" max="5" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.875" style="6"/>
+    <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="21" t="s">
         <v>121</v>
       </c>
@@ -2678,8 +2678,14 @@
       <c r="D2" s="24" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>25</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="22" t="s">
         <v>130</v>
       </c>
@@ -2692,8 +2698,14 @@
       <c r="D3" s="24" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>25</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>133</v>
       </c>
@@ -2703,11 +2715,17 @@
       <c r="C4" s="24" t="s">
         <v>181</v>
       </c>
-      <c r="D4" s="24" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D4" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>136</v>
       </c>
@@ -2720,8 +2738,14 @@
       <c r="D5" s="24" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>22</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>140</v>
       </c>
@@ -2731,11 +2755,17 @@
       <c r="C6" s="24" t="s">
         <v>182</v>
       </c>
-      <c r="D6" s="24" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D6" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="E6">
+        <v>20</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>145</v>
       </c>
@@ -2748,8 +2778,14 @@
       <c r="D7" s="24" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>160</v>
       </c>
@@ -2762,8 +2798,14 @@
       <c r="D8" s="24" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>15</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>119</v>
       </c>
@@ -2776,8 +2818,14 @@
       <c r="D9" s="24" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>20</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>120</v>
       </c>
@@ -2790,8 +2838,14 @@
       <c r="D10" s="24" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <v>20</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>122</v>
       </c>
@@ -2804,8 +2858,14 @@
       <c r="D11" s="24" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <v>20</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="26" t="s">
         <v>193</v>
       </c>
@@ -2813,44 +2873,40 @@
         <v>193</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B14" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B15" s="5"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B16" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B18" s="28" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B20" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B21" s="28" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B22" s="28" t="s">
-        <v>197</v>
-      </c>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B21" s="28"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B22" s="28"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2867,9 +2923,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2913,9 +2969,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -2958,9 +3014,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3003,13 +3059,13 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>118</v>
       </c>
@@ -3020,7 +3076,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A2" s="17" t="s">
         <v>119</v>
       </c>
@@ -3031,7 +3087,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
         <v>120</v>
       </c>
@@ -3042,7 +3098,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A4" s="17" t="s">
         <v>121</v>
       </c>
@@ -3053,7 +3109,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A5" s="17" t="s">
         <v>122</v>
       </c>
@@ -3064,7 +3120,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>123</v>
       </c>
@@ -3075,7 +3131,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>124</v>
       </c>
@@ -3086,7 +3142,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="48" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>125</v>
       </c>
@@ -3097,7 +3153,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>126</v>
       </c>
@@ -3108,7 +3164,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>127</v>
       </c>
@@ -3119,7 +3175,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>128</v>
       </c>
@@ -3130,7 +3186,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>129</v>
       </c>
@@ -3141,7 +3197,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="48" x14ac:dyDescent="0.15">
       <c r="A13" s="17" t="s">
         <v>130</v>
       </c>
@@ -3152,7 +3208,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="64" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>131</v>
       </c>
@@ -3163,7 +3219,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>132</v>
       </c>
@@ -3174,7 +3230,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A16" s="17" t="s">
         <v>133</v>
       </c>
@@ -3185,7 +3241,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>134</v>
       </c>
@@ -3196,7 +3252,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>135</v>
       </c>
@@ -3207,7 +3263,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A19" s="17" t="s">
         <v>136</v>
       </c>
@@ -3218,7 +3274,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>137</v>
       </c>
@@ -3229,7 +3285,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>138</v>
       </c>
@@ -3240,7 +3296,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>139</v>
       </c>
@@ -3251,7 +3307,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A23" s="17" t="s">
         <v>140</v>
       </c>
@@ -3262,7 +3318,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>141</v>
       </c>
@@ -3273,7 +3329,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="48" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>142</v>
       </c>
@@ -3284,7 +3340,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>143</v>
       </c>
@@ -3295,7 +3351,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="126" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="128" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>144</v>
       </c>
@@ -3306,7 +3362,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A28" s="17" t="s">
         <v>145</v>
       </c>
@@ -3317,7 +3373,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A29" s="24" t="s">
         <v>146</v>
       </c>
@@ -3328,7 +3384,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>147</v>
       </c>
@@ -3339,7 +3395,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>148</v>
       </c>
@@ -3350,7 +3406,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>149</v>
       </c>
@@ -3361,7 +3417,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>150</v>
       </c>
@@ -3372,7 +3428,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>151</v>
       </c>
@@ -3383,7 +3439,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="48" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>152</v>
       </c>
@@ -3394,7 +3450,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>153</v>
       </c>
@@ -3405,7 +3461,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>154</v>
       </c>
@@ -3416,7 +3472,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>155</v>
       </c>
@@ -3427,7 +3483,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>156</v>
       </c>
@@ -3438,7 +3494,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>157</v>
       </c>
@@ -3449,7 +3505,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>158</v>
       </c>
@@ -3460,7 +3516,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>159</v>
       </c>
@@ -3471,7 +3527,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A43" s="17" t="s">
         <v>160</v>
       </c>

</xml_diff>

<commit_message>
Updated my sprint status
</commit_message>
<xml_diff>
--- a/SSW_555/TeamPraRobSud555.xlsx
+++ b/SSW_555/TeamPraRobSud555.xlsx
@@ -5,7 +5,7 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sudhansh/git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sudhansh/git/SSW_555/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1050,11 +1050,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1116622048"/>
-        <c:axId val="1116624368"/>
+        <c:axId val="1568386016"/>
+        <c:axId val="1666295152"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="1116622048"/>
+        <c:axId val="1568386016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1064,14 +1064,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1116624368"/>
+        <c:crossAx val="1666295152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="1116624368"/>
+        <c:axId val="1666295152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1082,7 +1082,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1116622048"/>
+        <c:crossAx val="1568386016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1169,11 +1169,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1116664880"/>
-        <c:axId val="1116667632"/>
+        <c:axId val="1667306080"/>
+        <c:axId val="1667308896"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="1116664880"/>
+        <c:axId val="1667306080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1183,14 +1183,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1116667632"/>
+        <c:crossAx val="1667308896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="1116667632"/>
+        <c:axId val="1667308896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1201,7 +1201,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1116664880"/>
+        <c:crossAx val="1667306080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1238,7 +1238,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1276,7 +1276,7 @@
         <xdr:cNvPr id="3" name="Rectangular Callout 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1351,7 +1351,7 @@
         <xdr:cNvPr id="4" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1416,7 +1416,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1485,7 +1485,7 @@
         <xdr:cNvPr id="6" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1555,7 +1555,7 @@
         <xdr:cNvPr id="7" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1624,7 +1624,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1694,7 +1694,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2621,7 +2621,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2735,14 +2735,23 @@
       <c r="C5" s="24" t="s">
         <v>182</v>
       </c>
-      <c r="D5" s="24" t="s">
-        <v>195</v>
+      <c r="D5" s="29" t="s">
+        <v>197</v>
       </c>
       <c r="E5">
         <v>22</v>
       </c>
       <c r="F5">
         <v>2</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5" s="6">
+        <v>41329</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
@@ -2764,6 +2773,15 @@
       <c r="F6">
         <v>3</v>
       </c>
+      <c r="G6">
+        <v>6</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6" s="6">
+        <v>41322</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
@@ -2795,14 +2813,23 @@
       <c r="C8" s="24" t="s">
         <v>182</v>
       </c>
-      <c r="D8" s="24" t="s">
-        <v>195</v>
+      <c r="D8" s="29" t="s">
+        <v>197</v>
       </c>
       <c r="E8">
         <v>15</v>
       </c>
       <c r="F8">
         <v>2</v>
+      </c>
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8" s="6">
+        <v>41330</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
@@ -3055,8 +3082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="A18" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>